<commit_message>
Add default position and department
</commit_message>
<xml_diff>
--- a/ver1/src/main/resources/static/data.xlsx
+++ b/ver1/src/main/resources/static/data.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\hha management\backend\ver1\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D424A3-79FF-433B-8EB7-1F89CF5351E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25F0AC5-1537-4775-A06A-EF82982E42E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="1" xr2:uid="{E6CB9799-6C98-4C1B-939B-FC0F19C46569}"/>
   </bookViews>
   <sheets>
     <sheet name="account" sheetId="1" r:id="rId1"/>
     <sheet name="brand" sheetId="2" r:id="rId2"/>
+    <sheet name="position" sheetId="3" r:id="rId3"/>
+    <sheet name="department" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="323">
   <si>
     <t>Tiền mặt</t>
   </si>
@@ -797,13 +799,211 @@
   </si>
   <si>
     <t>Sweden</t>
+  </si>
+  <si>
+    <t>Director </t>
+  </si>
+  <si>
+    <t>Giám đốc</t>
+  </si>
+  <si>
+    <t>Vice Director</t>
+  </si>
+  <si>
+    <t>Chief Executive Officer (CEO)</t>
+  </si>
+  <si>
+    <t>Giám đốc điều hành</t>
+  </si>
+  <si>
+    <t>Chief Information Officer (CIO)</t>
+  </si>
+  <si>
+    <t>Giám đốc thông tin</t>
+  </si>
+  <si>
+    <t>Chief Operating Officer (COO)</t>
+  </si>
+  <si>
+    <t>Trưởng phòng hoạt động</t>
+  </si>
+  <si>
+    <t>Board of Directors</t>
+  </si>
+  <si>
+    <t>Hội đồng quản trị</t>
+  </si>
+  <si>
+    <t>Share holder</t>
+  </si>
+  <si>
+    <t>Cổ đông</t>
+  </si>
+  <si>
+    <t>Founder</t>
+  </si>
+  <si>
+    <t>Người sáng lập</t>
+  </si>
+  <si>
+    <t>Chủ tịch</t>
+  </si>
+  <si>
+    <t>Chairman</t>
+  </si>
+  <si>
+    <t>Vice president </t>
+  </si>
+  <si>
+    <t>Phó chủ tịch</t>
+  </si>
+  <si>
+    <t>Manager </t>
+  </si>
+  <si>
+    <t>Quản lý</t>
+  </si>
+  <si>
+    <t>Department manager </t>
+  </si>
+  <si>
+    <t>Trưởng phòng</t>
+  </si>
+  <si>
+    <t>Section manager</t>
+  </si>
+  <si>
+    <t>Supervisor </t>
+  </si>
+  <si>
+    <t>Người giám sát</t>
+  </si>
+  <si>
+    <t>Team Leader </t>
+  </si>
+  <si>
+    <t>Trưởng Nhóm</t>
+  </si>
+  <si>
+    <t>Assistant </t>
+  </si>
+  <si>
+    <t>Trợ lí giám đốc</t>
+  </si>
+  <si>
+    <t>Secretary </t>
+  </si>
+  <si>
+    <t>Thư kí</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Purchasing</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>R &amp; D</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Employee </t>
+  </si>
+  <si>
+    <t>Expert </t>
+  </si>
+  <si>
+    <t>Chuyên viên</t>
+  </si>
+  <si>
+    <t>Collaborator </t>
+  </si>
+  <si>
+    <t>Cộng tác viên</t>
+  </si>
+  <si>
+    <t>Trainee </t>
+  </si>
+  <si>
+    <t>Thực tập sinh</t>
+  </si>
+  <si>
+    <t>Apprentice </t>
+  </si>
+  <si>
+    <t>Người học việc</t>
+  </si>
+  <si>
+    <t>Team leader </t>
+  </si>
+  <si>
+    <t>Boss </t>
+  </si>
+  <si>
+    <t>Sếp</t>
+  </si>
+  <si>
+    <t>Receptionist </t>
+  </si>
+  <si>
+    <t>Nhân viên lễ tân</t>
+  </si>
+  <si>
+    <t>Officer </t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
+  </si>
+  <si>
+    <t>Phó giám đốc</t>
+  </si>
+  <si>
+    <t>Trưởng bộ phận</t>
+  </si>
+  <si>
+    <t>Hành chính</t>
+  </si>
+  <si>
+    <t>Nhân sự</t>
+  </si>
+  <si>
+    <t>Kinh doanh</t>
+  </si>
+  <si>
+    <t>Mua sắm vật tư</t>
+  </si>
+  <si>
+    <t>Nghiên cứu và phát triển</t>
+  </si>
+  <si>
+    <t>Vận chuyển</t>
+  </si>
+  <si>
+    <t>Kế toán</t>
+  </si>
+  <si>
+    <t>Tài chính</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -861,8 +1061,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -872,6 +1085,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0F0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -888,7 +1113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -906,6 +1131,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3828,13 +4065,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17171960-875D-4801-A484-B6F071940C9C}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A25" sqref="A1:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="15.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -4029,7 +4267,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>238</v>
       </c>
@@ -4115,6 +4353,319 @@
       </c>
       <c r="B35" s="8" t="s">
         <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A01EC1-BD16-4135-AD3D-DEFBB95A1DDE}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC71AD37-D450-4D95-AC08-7A2E31C57656}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add column level > position sample
</commit_message>
<xml_diff>
--- a/ver1/src/main/resources/static/data.xlsx
+++ b/ver1/src/main/resources/static/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\hha management\backend\ver1\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25F0AC5-1537-4775-A06A-EF82982E42E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1DAA79-5225-477E-B6AA-54BB73DF777E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="1" xr2:uid="{E6CB9799-6C98-4C1B-939B-FC0F19C46569}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="2" xr2:uid="{E6CB9799-6C98-4C1B-939B-FC0F19C46569}"/>
   </bookViews>
   <sheets>
     <sheet name="account" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="316">
   <si>
     <t>Tiền mặt</t>
   </si>
@@ -828,18 +828,6 @@
     <t>Trưởng phòng hoạt động</t>
   </si>
   <si>
-    <t>Board of Directors</t>
-  </si>
-  <si>
-    <t>Hội đồng quản trị</t>
-  </si>
-  <si>
-    <t>Share holder</t>
-  </si>
-  <si>
-    <t>Cổ đông</t>
-  </si>
-  <si>
     <t>Founder</t>
   </si>
   <si>
@@ -951,19 +939,10 @@
     <t>Team leader </t>
   </si>
   <si>
-    <t>Boss </t>
-  </si>
-  <si>
-    <t>Sếp</t>
-  </si>
-  <si>
     <t>Receptionist </t>
   </si>
   <si>
     <t>Nhân viên lễ tân</t>
-  </si>
-  <si>
-    <t>Officer </t>
   </si>
   <si>
     <t>Nhân viên</t>
@@ -4065,7 +4044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17171960-875D-4801-A484-B6F071940C9C}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A25" sqref="A1:B35"/>
     </sheetView>
   </sheetViews>
@@ -4362,10 +4341,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A01EC1-BD16-4135-AD3D-DEFBB95A1DDE}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4374,148 +4353,202 @@
     <col min="2" max="2" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>257</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>259</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>260</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>262</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>264</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>266</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>274</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>276</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="B13" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>281</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>283</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>285</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>286</v>
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>288</v>
+      <c r="A17" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>312</v>
+      <c r="C18">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -4525,6 +4558,9 @@
       <c r="B19" s="11" t="s">
         <v>299</v>
       </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
@@ -4533,57 +4569,34 @@
       <c r="B20" s="10" t="s">
         <v>301</v>
       </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>302</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="B22" s="11" t="s">
         <v>304</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>305</v>
+      <c r="C22">
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>309</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C27" s="11"/>
+      <c r="C23" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4606,66 +4619,66 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add branch id =1
</commit_message>
<xml_diff>
--- a/ver1/src/main/resources/static/data.xlsx
+++ b/ver1/src/main/resources/static/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\hha management\backend\ver1\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1DAA79-5225-477E-B6AA-54BB73DF777E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A616FFB-E029-4D7D-8DA3-24450F62C96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="2" xr2:uid="{E6CB9799-6C98-4C1B-939B-FC0F19C46569}"/>
   </bookViews>
@@ -903,12 +903,6 @@
     <t>Shipping</t>
   </si>
   <si>
-    <t>R &amp; D</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
     <t>Employee </t>
   </si>
   <si>
@@ -976,6 +970,12 @@
   </si>
   <si>
     <t>Tài chính</t>
+  </si>
+  <si>
+    <t>Human Resources</t>
+  </si>
+  <si>
+    <t>Research &amp; Development</t>
   </si>
 </sst>
 </file>
@@ -4343,14 +4343,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A01EC1-BD16-4135-AD3D-DEFBB95A1DDE}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -4369,7 +4370,7 @@
         <v>259</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -4468,7 +4469,7 @@
         <v>276</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -4520,10 +4521,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C16">
         <v>9</v>
@@ -4531,10 +4532,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -4542,10 +4543,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -4553,10 +4554,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -4564,10 +4565,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -4575,7 +4576,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>280</v>
@@ -4586,10 +4587,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C22">
         <v>9</v>
@@ -4605,80 +4606,105 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC71AD37-D450-4D95-AC08-7A2E31C57656}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:B8"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>285</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>286</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>287</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+        <v>307</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>288</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+        <v>308</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>289</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+        <v>309</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>291</v>
+        <v>315</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>290</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix default branch, add code
</commit_message>
<xml_diff>
--- a/ver1/src/main/resources/static/data.xlsx
+++ b/ver1/src/main/resources/static/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\hha management\backend\ver1\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C318DA37-AA60-473A-A8A3-BB431A9EF6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC5F7EF-713D-4B45-BAB7-0BD971400630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" activeTab="3" xr2:uid="{E6CB9799-6C98-4C1B-939B-FC0F19C46569}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="347">
   <si>
     <t>Tiền mặt</t>
   </si>
@@ -994,13 +994,88 @@
   </si>
   <si>
     <t>Ban lãnh đạo</t>
+  </si>
+  <si>
+    <t>Intern Techonogy</t>
+  </si>
+  <si>
+    <t>Board of Directors</t>
+  </si>
+  <si>
+    <t>RAD</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>SALES</t>
+  </si>
+  <si>
+    <t>Customer Services</t>
+  </si>
+  <si>
+    <t>Chăm sóc khách hàng</t>
+  </si>
+  <si>
+    <t>CSKH</t>
+  </si>
+  <si>
+    <t>PUR</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>FINANC</t>
+  </si>
+  <si>
+    <t>ACCOUNT</t>
+  </si>
+  <si>
+    <t>DELIVER</t>
+  </si>
+  <si>
+    <t>Treasury </t>
+  </si>
+  <si>
+    <t>Ngân quỹ</t>
+  </si>
+  <si>
+    <t>TREA</t>
+  </si>
+  <si>
+    <t>Product development</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Phát triển sản phẩm</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>Labor union</t>
+  </si>
+  <si>
+    <t>Công đoàn</t>
+  </si>
+  <si>
+    <t>LU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1071,6 +1146,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="BeVietnam-Regular.ttf"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1110,7 +1190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1141,6 +1221,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1461,14 +1542,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.75" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="1">
         <v>111</v>
       </c>
@@ -1479,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="3">
         <v>1111</v>
       </c>
@@ -1490,7 +1571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>1112</v>
       </c>
@@ -1501,7 +1582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="3">
         <v>1113</v>
       </c>
@@ -1512,7 +1593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="4">
         <v>112</v>
       </c>
@@ -1523,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="3">
         <v>1121</v>
       </c>
@@ -1534,7 +1615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="3">
         <v>1122</v>
       </c>
@@ -1545,7 +1626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="3">
         <v>1123</v>
       </c>
@@ -1556,7 +1637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="15.75">
       <c r="A9" s="4">
         <v>113</v>
       </c>
@@ -1567,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="3">
         <v>1131</v>
       </c>
@@ -1578,7 +1659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="3">
         <v>1132</v>
       </c>
@@ -1589,7 +1670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="15.75">
       <c r="A12" s="4">
         <v>121</v>
       </c>
@@ -1600,7 +1681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="3">
         <v>1211</v>
       </c>
@@ -1611,7 +1692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="3">
         <v>1212</v>
       </c>
@@ -1622,7 +1703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="3">
         <v>1218</v>
       </c>
@@ -1633,7 +1714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15.75">
       <c r="A16" s="4">
         <v>128</v>
       </c>
@@ -1644,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="3">
         <v>1281</v>
       </c>
@@ -1655,7 +1736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="3">
         <v>1282</v>
       </c>
@@ -1666,7 +1747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="3">
         <v>1283</v>
       </c>
@@ -1677,7 +1758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="3">
         <v>1288</v>
       </c>
@@ -1688,7 +1769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15.75">
       <c r="A21" s="4">
         <v>131</v>
       </c>
@@ -1699,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15.75">
       <c r="A22" s="4">
         <v>133</v>
       </c>
@@ -1710,7 +1791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" s="3">
         <v>1331</v>
       </c>
@@ -1721,7 +1802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" s="3">
         <v>1332</v>
       </c>
@@ -1732,7 +1813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15.75">
       <c r="A25" s="4">
         <v>136</v>
       </c>
@@ -1743,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" s="3">
         <v>1361</v>
       </c>
@@ -1754,7 +1835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" s="3">
         <v>1362</v>
       </c>
@@ -1765,7 +1846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="30">
       <c r="A28" s="3">
         <v>1363</v>
       </c>
@@ -1776,7 +1857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" s="3">
         <v>1368</v>
       </c>
@@ -1787,7 +1868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75">
       <c r="A30" s="4">
         <v>138</v>
       </c>
@@ -1798,7 +1879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" s="3">
         <v>1381</v>
       </c>
@@ -1809,7 +1890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" s="3">
         <v>1385</v>
       </c>
@@ -1820,7 +1901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" s="3">
         <v>1388</v>
       </c>
@@ -1831,7 +1912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="15.75">
       <c r="A34" s="4">
         <v>141</v>
       </c>
@@ -1842,7 +1923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="15.75">
       <c r="A35" s="4">
         <v>151</v>
       </c>
@@ -1853,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="15.75">
       <c r="A36" s="4">
         <v>152</v>
       </c>
@@ -1864,7 +1945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15.75">
       <c r="A37" s="4">
         <v>153</v>
       </c>
@@ -1875,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" s="3">
         <v>1531</v>
       </c>
@@ -1886,7 +1967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" s="3">
         <v>1532</v>
       </c>
@@ -1897,7 +1978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" s="3">
         <v>1533</v>
       </c>
@@ -1908,7 +1989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" s="3">
         <v>1534</v>
       </c>
@@ -1919,7 +2000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="15.75">
       <c r="A42" s="4">
         <v>154</v>
       </c>
@@ -1930,7 +2011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="15.75">
       <c r="A43" s="4">
         <v>155</v>
       </c>
@@ -1941,7 +2022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44" s="3">
         <v>1551</v>
       </c>
@@ -1952,7 +2033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45" s="3">
         <v>1557</v>
       </c>
@@ -1963,7 +2044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="15.75">
       <c r="A46" s="4">
         <v>156</v>
       </c>
@@ -1974,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47" s="3">
         <v>1561</v>
       </c>
@@ -1985,7 +2066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48" s="3">
         <v>1562</v>
       </c>
@@ -1996,7 +2077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3">
       <c r="A49" s="3">
         <v>1567</v>
       </c>
@@ -2007,7 +2088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="15.75">
       <c r="A50" s="4">
         <v>157</v>
       </c>
@@ -2018,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="15.75">
       <c r="A51" s="4">
         <v>158</v>
       </c>
@@ -2029,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="15.75">
       <c r="A52" s="4">
         <v>161</v>
       </c>
@@ -2040,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3">
       <c r="A53" s="3">
         <v>1611</v>
       </c>
@@ -2051,7 +2132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3">
       <c r="A54" s="3">
         <v>1612</v>
       </c>
@@ -2062,7 +2143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="15.75">
       <c r="A55" s="4">
         <v>171</v>
       </c>
@@ -2073,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="15.75">
       <c r="A56" s="4">
         <v>211</v>
       </c>
@@ -2084,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3">
       <c r="A57" s="3">
         <v>2111</v>
       </c>
@@ -2095,7 +2176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3">
       <c r="A58" s="3">
         <v>2112</v>
       </c>
@@ -2106,7 +2187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3">
       <c r="A59" s="3">
         <v>2113</v>
       </c>
@@ -2117,7 +2198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3">
       <c r="A60" s="3">
         <v>2114</v>
       </c>
@@ -2128,7 +2209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3">
       <c r="A61" s="3">
         <v>2115</v>
       </c>
@@ -2139,7 +2220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3">
       <c r="A62" s="3">
         <v>2118</v>
       </c>
@@ -2150,7 +2231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="15.75">
       <c r="A63" s="4">
         <v>212</v>
       </c>
@@ -2161,7 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3">
       <c r="A64" s="3">
         <v>2121</v>
       </c>
@@ -2172,7 +2253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3">
       <c r="A65" s="3">
         <v>2122</v>
       </c>
@@ -2183,7 +2264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="15.75">
       <c r="A66" s="4">
         <v>213</v>
       </c>
@@ -2194,7 +2275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3">
       <c r="A67" s="3">
         <v>2131</v>
       </c>
@@ -2205,7 +2286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3">
       <c r="A68" s="3">
         <v>2132</v>
       </c>
@@ -2216,7 +2297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3">
       <c r="A69" s="3">
         <v>2133</v>
       </c>
@@ -2227,7 +2308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3">
       <c r="A70" s="3">
         <v>2134</v>
       </c>
@@ -2238,7 +2319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3">
       <c r="A71" s="3">
         <v>2135</v>
       </c>
@@ -2249,7 +2330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3">
       <c r="A72" s="3">
         <v>2136</v>
       </c>
@@ -2260,7 +2341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3">
       <c r="A73" s="3">
         <v>2138</v>
       </c>
@@ -2271,7 +2352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="15.75">
       <c r="A74" s="4">
         <v>214</v>
       </c>
@@ -2282,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3">
       <c r="A75" s="3">
         <v>2141</v>
       </c>
@@ -2293,7 +2374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3">
       <c r="A76" s="3">
         <v>2142</v>
       </c>
@@ -2304,7 +2385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3">
       <c r="A77" s="3">
         <v>2143</v>
       </c>
@@ -2315,7 +2396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3">
       <c r="A78" s="3">
         <v>2147</v>
       </c>
@@ -2326,7 +2407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" ht="15.75">
       <c r="A79" s="4">
         <v>217</v>
       </c>
@@ -2337,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="15.75">
       <c r="A80" s="4">
         <v>221</v>
       </c>
@@ -2348,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="15.75">
       <c r="A81" s="4">
         <v>222</v>
       </c>
@@ -2359,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="15.75">
       <c r="A82" s="4">
         <v>228</v>
       </c>
@@ -2370,7 +2451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3">
       <c r="A83" s="3">
         <v>2281</v>
       </c>
@@ -2381,7 +2462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3">
       <c r="A84" s="3">
         <v>2288</v>
       </c>
@@ -2392,7 +2473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="15.75">
       <c r="A85" s="4">
         <v>229</v>
       </c>
@@ -2403,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3">
       <c r="A86" s="3">
         <v>2291</v>
       </c>
@@ -2414,7 +2495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3">
       <c r="A87" s="3">
         <v>2292</v>
       </c>
@@ -2425,7 +2506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3">
       <c r="A88" s="3">
         <v>2293</v>
       </c>
@@ -2436,7 +2517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3">
       <c r="A89" s="3">
         <v>2294</v>
       </c>
@@ -2447,7 +2528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="15.75">
       <c r="A90" s="4">
         <v>241</v>
       </c>
@@ -2458,7 +2539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3">
       <c r="A91" s="3">
         <v>2411</v>
       </c>
@@ -2469,7 +2550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3">
       <c r="A92" s="3">
         <v>2412</v>
       </c>
@@ -2480,7 +2561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3">
       <c r="A93" s="3">
         <v>2413</v>
       </c>
@@ -2491,7 +2572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="15.75">
       <c r="A94" s="4">
         <v>242</v>
       </c>
@@ -2502,7 +2583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="15.75">
       <c r="A95" s="4">
         <v>243</v>
       </c>
@@ -2513,7 +2594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="15.75">
       <c r="A96" s="4">
         <v>244</v>
       </c>
@@ -2524,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="15.75">
       <c r="A97" s="4">
         <v>331</v>
       </c>
@@ -2535,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" ht="15.75">
       <c r="A98" s="4">
         <v>333</v>
       </c>
@@ -2546,7 +2627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3">
       <c r="A99" s="3">
         <v>3331</v>
       </c>
@@ -2557,7 +2638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3">
       <c r="A100" s="3">
         <v>33311</v>
       </c>
@@ -2568,7 +2649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3">
       <c r="A101" s="3">
         <v>33312</v>
       </c>
@@ -2579,7 +2660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3">
       <c r="A102" s="3">
         <v>3332</v>
       </c>
@@ -2590,7 +2671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3">
       <c r="A103" s="3">
         <v>3333</v>
       </c>
@@ -2601,7 +2682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3">
       <c r="A104" s="3">
         <v>3334</v>
       </c>
@@ -2612,7 +2693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3">
       <c r="A105" s="3">
         <v>3335</v>
       </c>
@@ -2623,7 +2704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3">
       <c r="A106" s="3">
         <v>3336</v>
       </c>
@@ -2634,7 +2715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3">
       <c r="A107" s="3">
         <v>3337</v>
       </c>
@@ -2645,7 +2726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3">
       <c r="A108" s="3">
         <v>3338</v>
       </c>
@@ -2656,7 +2737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3">
       <c r="A109" s="3">
         <v>33381</v>
       </c>
@@ -2667,7 +2748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3">
       <c r="A110" s="3">
         <v>33382</v>
       </c>
@@ -2678,7 +2759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3">
       <c r="A111" s="3">
         <v>3339</v>
       </c>
@@ -2689,7 +2770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="15.75">
       <c r="A112" s="4">
         <v>334</v>
       </c>
@@ -2700,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3">
       <c r="A113" s="3">
         <v>3341</v>
       </c>
@@ -2711,7 +2792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3">
       <c r="A114" s="3">
         <v>3348</v>
       </c>
@@ -2722,7 +2803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" ht="15.75">
       <c r="A115" s="4">
         <v>335</v>
       </c>
@@ -2733,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" ht="15.75">
       <c r="A116" s="4">
         <v>336</v>
       </c>
@@ -2744,7 +2825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3">
       <c r="A117" s="3">
         <v>3361</v>
       </c>
@@ -2755,7 +2836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3">
       <c r="A118" s="3">
         <v>3362</v>
       </c>
@@ -2766,7 +2847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" ht="30">
       <c r="A119" s="3">
         <v>3363</v>
       </c>
@@ -2777,7 +2858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3">
       <c r="A120" s="3">
         <v>3368</v>
       </c>
@@ -2788,7 +2869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" ht="15.75">
       <c r="A121" s="4">
         <v>337</v>
       </c>
@@ -2799,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" ht="15.75">
       <c r="A122" s="4">
         <v>338</v>
       </c>
@@ -2810,7 +2891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3">
       <c r="A123" s="3">
         <v>3381</v>
       </c>
@@ -2821,7 +2902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3">
       <c r="A124" s="3">
         <v>3382</v>
       </c>
@@ -2832,7 +2913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3">
       <c r="A125" s="3">
         <v>3383</v>
       </c>
@@ -2843,7 +2924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3">
       <c r="A126" s="3">
         <v>3384</v>
       </c>
@@ -2854,7 +2935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3">
       <c r="A127" s="3">
         <v>3385</v>
       </c>
@@ -2865,7 +2946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3">
       <c r="A128" s="3">
         <v>3386</v>
       </c>
@@ -2876,7 +2957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3">
       <c r="A129" s="3">
         <v>3387</v>
       </c>
@@ -2887,7 +2968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3">
       <c r="A130" s="3">
         <v>3388</v>
       </c>
@@ -2898,7 +2979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" ht="15.75">
       <c r="A131" s="4">
         <v>341</v>
       </c>
@@ -2909,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3">
       <c r="A132" s="3">
         <v>3411</v>
       </c>
@@ -2920,7 +3001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3">
       <c r="A133" s="3">
         <v>3412</v>
       </c>
@@ -2931,7 +3012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="15.75">
       <c r="A134" s="4">
         <v>343</v>
       </c>
@@ -2942,7 +3023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3">
       <c r="A135" s="3">
         <v>3431</v>
       </c>
@@ -2953,7 +3034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3">
       <c r="A136" s="3">
         <v>34311</v>
       </c>
@@ -2964,7 +3045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3">
       <c r="A137" s="3">
         <v>34312</v>
       </c>
@@ -2975,7 +3056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3">
       <c r="A138" s="3">
         <v>34313</v>
       </c>
@@ -2986,7 +3067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3">
       <c r="A139" s="3">
         <v>3432</v>
       </c>
@@ -2997,7 +3078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" ht="15.75">
       <c r="A140" s="4">
         <v>344</v>
       </c>
@@ -3008,7 +3089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" ht="15.75">
       <c r="A141" s="4">
         <v>347</v>
       </c>
@@ -3019,7 +3100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" ht="15.75">
       <c r="A142" s="4">
         <v>352</v>
       </c>
@@ -3030,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3">
       <c r="A143" s="3">
         <v>3521</v>
       </c>
@@ -3041,7 +3122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3">
       <c r="A144" s="3">
         <v>3522</v>
       </c>
@@ -3052,7 +3133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3">
       <c r="A145" s="3">
         <v>3523</v>
       </c>
@@ -3063,7 +3144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3">
       <c r="A146" s="3">
         <v>3524</v>
       </c>
@@ -3074,7 +3155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" ht="15.75">
       <c r="A147" s="4">
         <v>353</v>
       </c>
@@ -3085,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3">
       <c r="A148" s="3">
         <v>3531</v>
       </c>
@@ -3096,7 +3177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3">
       <c r="A149" s="3">
         <v>3532</v>
       </c>
@@ -3107,7 +3188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3">
       <c r="A150" s="3">
         <v>3533</v>
       </c>
@@ -3118,7 +3199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3">
       <c r="A151" s="3">
         <v>3534</v>
       </c>
@@ -3129,7 +3210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" ht="15.75">
       <c r="A152" s="4">
         <v>356</v>
       </c>
@@ -3140,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3">
       <c r="A153" s="3">
         <v>3561</v>
       </c>
@@ -3151,7 +3232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" ht="30">
       <c r="A154" s="3">
         <v>3562</v>
       </c>
@@ -3162,7 +3243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" ht="15.75">
       <c r="A155" s="4">
         <v>357</v>
       </c>
@@ -3173,7 +3254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" ht="15.75">
       <c r="A156" s="4">
         <v>411</v>
       </c>
@@ -3184,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3">
       <c r="A157" s="3">
         <v>4111</v>
       </c>
@@ -3195,7 +3276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3">
       <c r="A158" s="3">
         <v>41111</v>
       </c>
@@ -3206,7 +3287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3">
       <c r="A159" s="3">
         <v>41112</v>
       </c>
@@ -3217,7 +3298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3">
       <c r="A160" s="3">
         <v>4112</v>
       </c>
@@ -3228,7 +3309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3">
       <c r="A161" s="3">
         <v>4113</v>
       </c>
@@ -3239,7 +3320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3">
       <c r="A162" s="3">
         <v>4118</v>
       </c>
@@ -3250,7 +3331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" ht="15.75">
       <c r="A163" s="4">
         <v>412</v>
       </c>
@@ -3261,7 +3342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" ht="15.75">
       <c r="A164" s="4">
         <v>413</v>
       </c>
@@ -3272,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" ht="30">
       <c r="A165" s="3">
         <v>4131</v>
       </c>
@@ -3283,7 +3364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" ht="30">
       <c r="A166" s="3">
         <v>4132</v>
       </c>
@@ -3294,7 +3375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" ht="15.75">
       <c r="A167" s="4">
         <v>414</v>
       </c>
@@ -3305,7 +3386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" ht="15.75">
       <c r="A168" s="4">
         <v>417</v>
       </c>
@@ -3316,7 +3397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" ht="15.75">
       <c r="A169" s="4">
         <v>418</v>
       </c>
@@ -3327,7 +3408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" ht="15.75">
       <c r="A170" s="4">
         <v>419</v>
       </c>
@@ -3338,7 +3419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" ht="15.75">
       <c r="A171" s="4">
         <v>421</v>
       </c>
@@ -3349,7 +3430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3">
       <c r="A172" s="3">
         <v>4211</v>
       </c>
@@ -3360,7 +3441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3">
       <c r="A173" s="3">
         <v>4212</v>
       </c>
@@ -3371,7 +3452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" ht="15.75">
       <c r="A174" s="4">
         <v>441</v>
       </c>
@@ -3382,7 +3463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" ht="15.75">
       <c r="A175" s="4">
         <v>461</v>
       </c>
@@ -3393,7 +3474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3">
       <c r="A176" s="3">
         <v>4611</v>
       </c>
@@ -3404,7 +3485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3">
       <c r="A177" s="3">
         <v>4612</v>
       </c>
@@ -3415,7 +3496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" ht="15.75">
       <c r="A178" s="4">
         <v>466</v>
       </c>
@@ -3426,7 +3507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" ht="15.75">
       <c r="A179" s="4">
         <v>511</v>
       </c>
@@ -3437,7 +3518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3">
       <c r="A180" s="3">
         <v>5111</v>
       </c>
@@ -3448,7 +3529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3">
       <c r="A181" s="3">
         <v>5112</v>
       </c>
@@ -3459,7 +3540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3">
       <c r="A182" s="3">
         <v>5113</v>
       </c>
@@ -3470,7 +3551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3">
       <c r="A183" s="3">
         <v>5114</v>
       </c>
@@ -3481,7 +3562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3">
       <c r="A184" s="3">
         <v>5117</v>
       </c>
@@ -3492,7 +3573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3">
       <c r="A185" s="3">
         <v>5118</v>
       </c>
@@ -3503,7 +3584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" ht="15.75">
       <c r="A186" s="4">
         <v>515</v>
       </c>
@@ -3514,7 +3595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" ht="15.75">
       <c r="A187" s="4">
         <v>521</v>
       </c>
@@ -3525,7 +3606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3">
       <c r="A188" s="3">
         <v>5211</v>
       </c>
@@ -3536,7 +3617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3">
       <c r="A189" s="3">
         <v>5212</v>
       </c>
@@ -3547,7 +3628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3">
       <c r="A190" s="3">
         <v>5213</v>
       </c>
@@ -3558,7 +3639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" ht="15.75">
       <c r="A191" s="4">
         <v>611</v>
       </c>
@@ -3569,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3">
       <c r="A192" s="3">
         <v>6111</v>
       </c>
@@ -3580,7 +3661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3">
       <c r="A193" s="3">
         <v>6112</v>
       </c>
@@ -3591,7 +3672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" ht="15.75">
       <c r="A194" s="4">
         <v>621</v>
       </c>
@@ -3602,7 +3683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" ht="15.75">
       <c r="A195" s="4">
         <v>622</v>
       </c>
@@ -3613,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" ht="15.75">
       <c r="A196" s="4">
         <v>623</v>
       </c>
@@ -3624,7 +3705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3">
       <c r="A197" s="3">
         <v>6231</v>
       </c>
@@ -3635,7 +3716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3">
       <c r="A198" s="3">
         <v>6232</v>
       </c>
@@ -3646,7 +3727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3">
       <c r="A199" s="3">
         <v>6233</v>
       </c>
@@ -3657,7 +3738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3">
       <c r="A200" s="3">
         <v>6234</v>
       </c>
@@ -3668,7 +3749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3">
       <c r="A201" s="3">
         <v>6237</v>
       </c>
@@ -3679,7 +3760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3">
       <c r="A202" s="3">
         <v>6238</v>
       </c>
@@ -3690,7 +3771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" ht="15.75">
       <c r="A203" s="4">
         <v>627</v>
       </c>
@@ -3701,7 +3782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3">
       <c r="A204" s="3">
         <v>6271</v>
       </c>
@@ -3712,7 +3793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3">
       <c r="A205" s="3">
         <v>6272</v>
       </c>
@@ -3723,7 +3804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3">
       <c r="A206" s="3">
         <v>6273</v>
       </c>
@@ -3734,7 +3815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3">
       <c r="A207" s="3">
         <v>6274</v>
       </c>
@@ -3745,7 +3826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3">
       <c r="A208" s="3">
         <v>6277</v>
       </c>
@@ -3756,7 +3837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3">
       <c r="A209" s="3">
         <v>6278</v>
       </c>
@@ -3767,7 +3848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" ht="15.75">
       <c r="A210" s="4">
         <v>631</v>
       </c>
@@ -3778,7 +3859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" ht="15.75">
       <c r="A211" s="4">
         <v>632</v>
       </c>
@@ -3789,7 +3870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" ht="15.75">
       <c r="A212" s="4">
         <v>635</v>
       </c>
@@ -3800,7 +3881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" ht="15.75">
       <c r="A213" s="4">
         <v>641</v>
       </c>
@@ -3811,7 +3892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3">
       <c r="A214" s="3">
         <v>6411</v>
       </c>
@@ -3822,7 +3903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3">
       <c r="A215" s="3">
         <v>6412</v>
       </c>
@@ -3833,7 +3914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3">
       <c r="A216" s="3">
         <v>6413</v>
       </c>
@@ -3844,7 +3925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3">
       <c r="A217" s="3">
         <v>6414</v>
       </c>
@@ -3855,7 +3936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3">
       <c r="A218" s="3">
         <v>6415</v>
       </c>
@@ -3866,7 +3947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3">
       <c r="A219" s="3">
         <v>6417</v>
       </c>
@@ -3877,7 +3958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3">
       <c r="A220" s="3">
         <v>6418</v>
       </c>
@@ -3888,7 +3969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" ht="15.75">
       <c r="A221" s="4">
         <v>642</v>
       </c>
@@ -3899,7 +3980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3">
       <c r="A222" s="3">
         <v>6421</v>
       </c>
@@ -3910,7 +3991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3">
       <c r="A223" s="3">
         <v>6422</v>
       </c>
@@ -3921,7 +4002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3">
       <c r="A224" s="3">
         <v>6423</v>
       </c>
@@ -3932,7 +4013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3">
       <c r="A225" s="3">
         <v>6424</v>
       </c>
@@ -3943,7 +4024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3">
       <c r="A226" s="3">
         <v>6425</v>
       </c>
@@ -3954,7 +4035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3">
       <c r="A227" s="3">
         <v>6426</v>
       </c>
@@ -3965,7 +4046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3">
       <c r="A228" s="3">
         <v>6427</v>
       </c>
@@ -3976,7 +4057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3">
       <c r="A229" s="3">
         <v>6428</v>
       </c>
@@ -3987,7 +4068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" ht="15.75">
       <c r="A230" s="4">
         <v>711</v>
       </c>
@@ -3998,7 +4079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" ht="15.75">
       <c r="A231" s="4">
         <v>811</v>
       </c>
@@ -4009,7 +4090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" ht="15.75">
       <c r="A232" s="4">
         <v>821</v>
       </c>
@@ -4020,7 +4101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3">
       <c r="A233" s="3">
         <v>8211</v>
       </c>
@@ -4031,7 +4112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3">
       <c r="A234" s="3">
         <v>8212</v>
       </c>
@@ -4042,7 +4123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" ht="15.75">
       <c r="A235" s="4">
         <v>911</v>
       </c>
@@ -4066,13 +4147,13 @@
       <selection activeCell="A25" sqref="A1:B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.375" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5">
       <c r="A1" s="7" t="s">
         <v>214</v>
       </c>
@@ -4080,7 +4161,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16.5">
       <c r="A2" s="9" t="s">
         <v>215</v>
       </c>
@@ -4088,7 +4169,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16.5">
       <c r="A3" s="9" t="s">
         <v>216</v>
       </c>
@@ -4096,7 +4177,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.5">
       <c r="A4" s="9" t="s">
         <v>217</v>
       </c>
@@ -4104,7 +4185,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="16.5">
       <c r="A5" s="9" t="s">
         <v>218</v>
       </c>
@@ -4112,7 +4193,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="16.5">
       <c r="A6" s="9" t="s">
         <v>219</v>
       </c>
@@ -4120,7 +4201,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="16.5">
       <c r="A7" s="9" t="s">
         <v>220</v>
       </c>
@@ -4128,7 +4209,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="16.5">
       <c r="A8" s="9" t="s">
         <v>221</v>
       </c>
@@ -4136,7 +4217,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="16.5">
       <c r="A9" s="9" t="s">
         <v>222</v>
       </c>
@@ -4144,7 +4225,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="16.5">
       <c r="A10" s="9" t="s">
         <v>223</v>
       </c>
@@ -4152,7 +4233,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="16.5">
       <c r="A11" s="9" t="s">
         <v>224</v>
       </c>
@@ -4160,7 +4241,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="16.5">
       <c r="A12" s="9" t="s">
         <v>225</v>
       </c>
@@ -4168,7 +4249,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="16.5">
       <c r="A13" s="9" t="s">
         <v>226</v>
       </c>
@@ -4176,7 +4257,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="16.5">
       <c r="A14" s="9" t="s">
         <v>227</v>
       </c>
@@ -4184,7 +4265,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="16.5">
       <c r="A15" s="9" t="s">
         <v>228</v>
       </c>
@@ -4192,7 +4273,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="16.5">
       <c r="A16" s="9" t="s">
         <v>229</v>
       </c>
@@ -4200,7 +4281,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="16.5">
       <c r="A17" s="9" t="s">
         <v>230</v>
       </c>
@@ -4208,7 +4289,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="16.5">
       <c r="A18" s="9" t="s">
         <v>231</v>
       </c>
@@ -4216,7 +4297,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="16.5">
       <c r="A19" s="9" t="s">
         <v>232</v>
       </c>
@@ -4224,7 +4305,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="16.5">
       <c r="A20" s="9" t="s">
         <v>233</v>
       </c>
@@ -4232,7 +4313,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="16.5">
       <c r="A21" s="9" t="s">
         <v>234</v>
       </c>
@@ -4240,7 +4321,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="16.5">
       <c r="A22" s="9" t="s">
         <v>235</v>
       </c>
@@ -4248,7 +4329,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="16.5">
       <c r="A23" s="9" t="s">
         <v>236</v>
       </c>
@@ -4256,7 +4337,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="16.5">
       <c r="A24" s="9" t="s">
         <v>237</v>
       </c>
@@ -4264,7 +4345,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="16.5">
       <c r="A25" s="9" t="s">
         <v>238</v>
       </c>
@@ -4272,7 +4353,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="16.5">
       <c r="A26" s="9" t="s">
         <v>239</v>
       </c>
@@ -4280,7 +4361,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="16.5">
       <c r="A27" s="9" t="s">
         <v>240</v>
       </c>
@@ -4288,7 +4369,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="16.5">
       <c r="A28" s="9" t="s">
         <v>241</v>
       </c>
@@ -4296,7 +4377,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="16.5">
       <c r="A29" s="9" t="s">
         <v>242</v>
       </c>
@@ -4304,7 +4385,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="16.5">
       <c r="A30" s="9" t="s">
         <v>243</v>
       </c>
@@ -4312,7 +4393,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="16.5">
       <c r="A31" s="9" t="s">
         <v>244</v>
       </c>
@@ -4320,7 +4401,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="16.5">
       <c r="A32" s="9" t="s">
         <v>245</v>
       </c>
@@ -4328,7 +4409,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="16.5">
       <c r="A33" s="9" t="s">
         <v>246</v>
       </c>
@@ -4336,7 +4417,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="16.5">
       <c r="A34" s="9" t="s">
         <v>247</v>
       </c>
@@ -4344,7 +4425,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="16.5">
       <c r="A35" s="9" t="s">
         <v>248</v>
       </c>
@@ -4365,14 +4446,14 @@
       <selection activeCell="A4" sqref="A4:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="26.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
         <v>257</v>
       </c>
@@ -4383,7 +4464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="10" t="s">
         <v>259</v>
       </c>
@@ -4394,7 +4475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="11" t="s">
         <v>260</v>
       </c>
@@ -4405,7 +4486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="10" t="s">
         <v>262</v>
       </c>
@@ -4416,7 +4497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
         <v>264</v>
       </c>
@@ -4427,7 +4508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="10" t="s">
         <v>266</v>
       </c>
@@ -4438,7 +4519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="10" t="s">
         <v>269</v>
       </c>
@@ -4449,7 +4530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="11" t="s">
         <v>270</v>
       </c>
@@ -4460,7 +4541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="10" t="s">
         <v>272</v>
       </c>
@@ -4471,7 +4552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="11" t="s">
         <v>274</v>
       </c>
@@ -4482,7 +4563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="10" t="s">
         <v>276</v>
       </c>
@@ -4493,7 +4574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="11" t="s">
         <v>277</v>
       </c>
@@ -4504,7 +4585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="10" t="s">
         <v>279</v>
       </c>
@@ -4515,7 +4596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="11" t="s">
         <v>281</v>
       </c>
@@ -4526,7 +4607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="10" t="s">
         <v>283</v>
       </c>
@@ -4537,7 +4618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="10" t="s">
         <v>291</v>
       </c>
@@ -4548,7 +4629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="11" t="s">
         <v>292</v>
       </c>
@@ -4559,7 +4640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="10" t="s">
         <v>294</v>
       </c>
@@ -4570,7 +4651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="11" t="s">
         <v>296</v>
       </c>
@@ -4581,7 +4662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="10" t="s">
         <v>298</v>
       </c>
@@ -4592,7 +4673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="11" t="s">
         <v>300</v>
       </c>
@@ -4603,7 +4684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="11" t="s">
         <v>301</v>
       </c>
@@ -4614,7 +4695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="C23" s="11"/>
     </row>
   </sheetData>
@@ -4624,20 +4705,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC71AD37-D450-4D95-AC08-7A2E31C57656}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="1.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="10" t="s">
         <v>285</v>
       </c>
@@ -4645,10 +4726,13 @@
         <v>312</v>
       </c>
       <c r="C1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="11" t="s">
         <v>286</v>
       </c>
@@ -4656,10 +4740,13 @@
         <v>313</v>
       </c>
       <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="10" t="s">
         <v>287</v>
       </c>
@@ -4667,10 +4754,13 @@
         <v>306</v>
       </c>
       <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="11" t="s">
         <v>314</v>
       </c>
@@ -4678,10 +4768,13 @@
         <v>307</v>
       </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="10" t="s">
         <v>288</v>
       </c>
@@ -4689,10 +4782,13 @@
         <v>308</v>
       </c>
       <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="11" t="s">
         <v>289</v>
       </c>
@@ -4700,10 +4796,13 @@
         <v>309</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.5">
       <c r="A7" s="10" t="s">
         <v>315</v>
       </c>
@@ -4711,10 +4810,13 @@
         <v>310</v>
       </c>
       <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="11" t="s">
         <v>290</v>
       </c>
@@ -4722,23 +4824,29 @@
         <v>311</v>
       </c>
       <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="10" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>317</v>
       </c>
       <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="11" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>319</v>
@@ -4746,8 +4854,11 @@
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="10" t="s">
         <v>320</v>
       </c>
@@ -4756,6 +4867,79 @@
       </c>
       <c r="C11">
         <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15">
+      <c r="A12" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15">
+      <c r="A13" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15">
+      <c r="A14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15">
+      <c r="A15" t="s">
+        <v>340</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15">
+      <c r="A16" t="s">
+        <v>344</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>